<commit_message>
Forgot to commit changes that include timezone adding and other stuff
</commit_message>
<xml_diff>
--- a/originals/Sol.xlsx
+++ b/originals/Sol.xlsx
@@ -2,25 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faerar\PycharmProjects\excl-TMZ\originals\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Faerar\Downloads\Assignment 2\Updated Records 2024-03-14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7352D3-0E86-4B00-93C4-2EE457E93708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{906112BD-5AD3-419A-B0BF-94B932213B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="7470" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="7470" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -6115,10 +6110,10 @@
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -6149,7 +6144,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -6172,44 +6167,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -6236,32 +6231,14 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -6288,24 +6265,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -6317,203 +6276,178 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="phClr"/>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD1902"/>
+  <dimension ref="A1:AD1901"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A1:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.140625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -89073,9 +89007,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="1902" spans="1:30" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>